<commit_message>
EM added ogp and colmex presentations
</commit_message>
<xml_diff>
--- a/papers/pygSpanish/Disponibilidad Info04.xlsx
+++ b/papers/pygSpanish/Disponibilidad Info04.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="66">
   <si>
     <t>Información</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Bases de datos</t>
   </si>
   <si>
-    <t>   Población </t>
+    <t>Población</t>
   </si>
   <si>
     <t>Datos</t>
@@ -81,19 +81,19 @@
     <t>INE-IENGI</t>
   </si>
   <si>
-    <t>   Población indígena</t>
+    <t>Población indígena</t>
   </si>
   <si>
     <t>CDI</t>
   </si>
   <si>
-    <t>   Vías de comunciación</t>
+    <t>Vías de comunciación</t>
   </si>
   <si>
     <t>SCT</t>
   </si>
   <si>
-    <t>   Tiempos de traslado</t>
+    <t>Tiempos de traslado</t>
   </si>
   <si>
     <t>✗</t>
@@ -105,19 +105,19 @@
     <t>INE</t>
   </si>
   <si>
-    <t>   Contigüidad geográfica</t>
+    <t>Contigüidad geográfica</t>
   </si>
   <si>
     <t>Software GIS</t>
   </si>
   <si>
-    <t>   Municipios únicos***</t>
+    <t>Municipios únicos***</t>
   </si>
   <si>
     <t>Cartografía</t>
   </si>
   <si>
-    <t>   Administrativa (estados, municipios)</t>
+    <t>Administrativa (estados, municipios)</t>
   </si>
   <si>
     <t>Sección</t>
@@ -126,16 +126,16 @@
     <t>INE-INEGI</t>
   </si>
   <si>
-    <t>   Accidentes geográficos</t>
+    <t>Accidentes geográficos</t>
   </si>
   <si>
     <t>INEGI</t>
   </si>
   <si>
-    <t>   División política federal</t>
-  </si>
-  <si>
-    <t>   División política local</t>
+    <t>División política federal</t>
+  </si>
+  <si>
+    <t>División política local</t>
   </si>
   <si>
     <r>
@@ -179,7 +179,7 @@
     <t>Texto</t>
   </si>
   <si>
-    <t>   Componentes del modelo </t>
+    <t>Componentes del modelo</t>
   </si>
   <si>
     <t>Software</t>
@@ -211,9 +211,6 @@
     </r>
   </si>
   <si>
-    <t>Software </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve"> Software </t>
     </r>
@@ -229,7 +226,7 @@
     </r>
   </si>
   <si>
-    <t>   Plataforma de indicadores </t>
+    <t>Plataforma de indicadores</t>
   </si>
   <si>
     <r>
@@ -250,28 +247,28 @@
     <t>Mapas y revisiones</t>
   </si>
   <si>
-    <t>   Escenarios automatizados</t>
+    <t>Escenarios automatizados</t>
   </si>
   <si>
     <t>Distrito-estado</t>
   </si>
   <si>
-    <t>   Escenarios partidistas</t>
+    <t>Escenarios partidistas</t>
   </si>
   <si>
     <t>INE-Partidos</t>
   </si>
   <si>
-    <t>   Justificación partidista</t>
-  </si>
-  <si>
-    <t>   Fallos del comité técnico</t>
+    <t>Justificación partidista</t>
+  </si>
+  <si>
+    <t>Fallos del comité técnico</t>
   </si>
   <si>
     <t>Normatividad</t>
   </si>
   <si>
-    <t>   Marco legal </t>
+    <t>Marco legal</t>
   </si>
   <si>
     <t>Resultados electorales</t>
@@ -349,8 +346,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> (la información no está en línea, pero la institución tiene un medio de distribución público), 
-</t>
+      <t xml:space="preserve"> (la información no está en línea, pero la institución tiene un medio de distribución público), </t>
     </r>
     <r>
       <rPr>
@@ -369,7 +365,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> (la inforamación está disponible en línea). </t>
+      <t xml:space="preserve"> (la información está disponible en línea). </t>
     </r>
   </si>
   <si>
@@ -379,7 +375,7 @@
     <t>Notes on the Diagram</t>
   </si>
   <si>
-    <t>Seems that what we are talking of transparency in the table, relate to the Diagram (Table 1 satisfies transparency, but not participation). If you satisfy table one, Seems we should indicate where we are, and were this intervention would get us. Mexico is at level 3. In order to get to level 4, Table 1 is necessary. The redistricting and Technology (redistricting in the West, awerness, comentary. participation, being incorporated in the process). There is another level: 1) able to evealuate countreproposals and 2) can you comment on proposals and submit (informally)? 3) be part of the decission process formally? There needs to be something between 3 and 4 that says where we are and what the intervention does? The fifth level, seems odd. There is a difference between direct formal involvement in the process of redistricting and formal access to representation. </t>
+    <t>Seems that what we are talking of transparency in the table, relate to the Diagram (Table 1 satisfies transparency, but not participation). If you satisfy table one, Seems we should indicate where we are, and were this intervention would get us. Mexico is at level 3. In order to get to level 4, Table 1 is necessary. The redistricting and Technology (redistricting in the West, awerness, comentary. participation, being incorporated in the process). There is another level: 1) able to evealuate countreproposals and 2) can you comment on proposals and submit (informally)? 3) be part of the decission process formally? There needs to be something between 3 and 4 that says where we are and what the intervention does? The fifth level, seems odd. There is a difference between direct formal involvement in the process of redistricting and formal access to representation.</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1112,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>15</v>
@@ -1128,7 +1124,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>22</v>
@@ -1139,10 +1135,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>15</v>
@@ -1154,7 +1150,7 @@
         <v>37</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>22</v>
@@ -1165,10 +1161,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>15</v>
@@ -1180,7 +1176,7 @@
         <v>37</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>22</v>
@@ -1201,7 +1197,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -1213,13 +1209,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>22</v>
@@ -1239,13 +1235,13 @@
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>22</v>
@@ -1260,12 +1256,12 @@
         <v>12</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>41</v>
@@ -1286,12 +1282,12 @@
         <v>15</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>41</v>
@@ -1327,7 +1323,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
@@ -1339,7 +1335,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>41</v>
@@ -1375,7 +1371,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
@@ -1387,13 +1383,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>61</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>12</v>
@@ -1423,7 +1419,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -1433,9 +1429,9 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -1447,7 +1443,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -1507,14 +1503,17 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F45" s="0"/>
+    </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="554.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>